<commit_message>
added all new Documents and changed Systemtest
</commit_message>
<xml_diff>
--- a/Testdokumente/systemtest.xlsx
+++ b/Testdokumente/systemtest.xlsx
@@ -1,112 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tarik\OneDrive\Dokumente\Studium\5.Semester_WS1718\Projekt 2\Documentation\Testdokumente\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/varmahal/Library/Mobile Documents/com~apple~CloudDocs/yourChoice/Documentation/Testdokumente/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11028" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16220"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Tarik Bozdemir</author>
-  </authors>
-  <commentList>
-    <comment ref="E14" authorId="0" shapeId="0" xr:uid="{3232EA98-11D9-4674-ABC6-6A9AF08009C0}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tarik Bozdemir:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-"und ist somit […] zugänglich"</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E15" authorId="0" shapeId="0" xr:uid="{65BB8131-F77E-4C93-9944-F09C885E45AD}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tarik Bozdemir:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-"und ist somit [...] Fehlermeldung"</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D29" authorId="0" shapeId="0" xr:uid="{55F470DD-D4E7-423A-A966-A1FCDDB6B1D3}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Tarik Bozdemir:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-ist es richtig das bei 29 und 30 jeweils "Stimme mehrfach oder gar nicht abgeben steht"? Ist auch bei den folgenden so</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="124">
   <si>
     <t>Nr.</t>
   </si>
@@ -324,24 +248,9 @@
     <t>Bundestagswahl aus Liste der verfügbaren Wahlen auswählen -&gt; Erststimme abgeben -&gt; Zweitstimme abgeben -&gt; Button "Auswahl bestätigen" anklicken -&gt; Button "Ja" anklicken</t>
   </si>
   <si>
-    <t>Bundestagswahl aus Liste der verfügbaren Wahlen auswählen -&gt; Erststimme oder Zweitstimme abgeben  -&gt; Button "Auswahl bestätigen" anklicken -&gt; Button "Ja" anklicken</t>
-  </si>
-  <si>
-    <t>Bundestagswahl aus Liste der verfügbaren Wahlen auswählen -&gt; Erstimme und mehrfach Zweitstimme abgeben oder mehrfach Erststimme und Zweitstimme abgeben -&gt; Button "Auswahl bestätigen" anklicken -&gt; Button "Ja" anklicken</t>
-  </si>
-  <si>
     <t>Europawahl aus Liste der verfügbaren Wahlen auswählen -&gt; Stimme abgeben -&gt; Button "Auswahl bestätigen" anklicken -&gt; Button "Ja" anklicken</t>
   </si>
   <si>
-    <t>Europawahl aus Liste der verfügbaren Wahlen auswählen -&gt; Stimme mehrfach oder gar nicht abgeben -&gt; Button "Auswahl bestätigen" anklicken -&gt; Button "Ja" anklicken</t>
-  </si>
-  <si>
-    <t>Bürgerentscheid aus Liste der verfügbaren Wahlen auswählen -&gt; Stimme mehrfach oder gar nicht abgeben -&gt; Button "Auswahl bestätigen" anklicken -&gt; Button "Ja" anklicken</t>
-  </si>
-  <si>
-    <t>Landratswahl aus Liste der verfügbaren Wahlen auswählen -&gt; Stimme mehrfach oder gar nicht abgeben -&gt; Button "Auswahl bestätigen" anklicken -&gt; Button "Ja" anklicken</t>
-  </si>
-  <si>
     <t>Bürgermeisterwahl aus Liste der verfügbaren Wahlen auswählen -&gt; Stimme mehrfach oder gar nicht abgeben -&gt; Button "Auswahl bestätigen" anklicken -&gt; Button "Ja" anklicken</t>
   </si>
   <si>
@@ -468,36 +377,44 @@
     <t>Auswertung stimmt nicht und Möglichkeit einer Handauswertung (z.B. durch Ausdruck aus der Datenbank).</t>
   </si>
   <si>
-    <t>Wahl ist freigegeben und ist somit für die Wähler zugänglich. Es können weitere Wahlen freigegeben/gelöscht werden.</t>
-  </si>
-  <si>
-    <t>Wahl wurde abgelehnt und ist somit nicht für die Wähler zugänglich. Dialog Fenster öffnet sich mit Fehlermeldung. Es können weitere Wahlen freigegeben/gelöscht werden.</t>
+    <t>Bürgerentscheid aus Liste der verfügbaren Wahlen auswählen -&gt; Stimme abgeben -&gt; Button "Auswahl bestätigen" anklicken -&gt; Button "Ja" anklicken</t>
+  </si>
+  <si>
+    <t>Landratswahl aus Liste der verfügbaren Wahlen auswählen -&gt; Stimme abgeben -&gt; Button "Auswahl bestätigen" anklicken -&gt; Button "Ja" anklicken</t>
+  </si>
+  <si>
+    <t>Bundestagswahl aus Liste der verfügbaren Wahlen auswählen -&gt; Button "Stimme ungültig machen" anklicken -&gt; Button "Ja" anklicken</t>
+  </si>
+  <si>
+    <t>Europawahl aus Liste der verfügbaren Wahlen auswählen -&gt; Button "Stimme ungültig machen" anklicken -&gt; Button "Ja" anklicken</t>
+  </si>
+  <si>
+    <t>Bürgerentscheid aus Liste der verfügbaren Wahlen auswählen -&gt; Button "Stimme ungültig machen" anklicken -&gt; Button "Ja" anklicken</t>
+  </si>
+  <si>
+    <t>Landratswahl aus Liste der verfügbaren Wahlen auswählen -&gt; Button "Stimme ungültig machen" anklicken -&gt; Button "Ja" anklicken</t>
+  </si>
+  <si>
+    <t>Bürgermeisterwahl aus Liste der verfügbaren Wahlen auswählen -&gt; Button "Stimme ungültig machen" anklicken -&gt; Button "Ja" anklicken</t>
+  </si>
+  <si>
+    <t>Wahl ist freigegeben und ist somit ab dem entsprechenden Datum für die Wähler zugänglich. Es können weitere Wahlen freigegeben/gelöscht werden.</t>
+  </si>
+  <si>
+    <t>Wahl wurde abgelehnt. Moderator wird darüber informiert. Es können weitere Wahlen freigegeben/gelöscht werden.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -527,7 +444,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -554,7 +471,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -832,24 +749,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D25" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" zoomScale="41" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="50.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="91.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="71.88671875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.44140625" style="1"/>
+    <col min="2" max="2" width="35.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="91.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="71.83203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -866,7 +783,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -883,7 +800,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -900,7 +817,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -917,7 +834,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -934,109 +851,109 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -1047,13 +964,13 @@
         <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -1067,10 +984,10 @@
         <v>18</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -1087,7 +1004,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>14</v>
       </c>
@@ -1104,7 +1021,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>15</v>
       </c>
@@ -1121,7 +1038,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>16</v>
       </c>
@@ -1138,7 +1055,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>17</v>
       </c>
@@ -1149,185 +1066,185 @@
         <v>33</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>72</v>
+        <v>117</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>18</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>19</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>21</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
-        <v>20</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>23</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
-        <v>22</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>77</v>
+        <v>120</v>
       </c>
       <c r="E32" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>25</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
-        <v>24</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>78</v>
+        <v>121</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
-        <v>26</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E36" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>27</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>45</v>
@@ -1336,15 +1253,15 @@
         <v>47</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>45</v>
@@ -1353,49 +1270,49 @@
         <v>47</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A41" s="1">
-        <v>30</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E41" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>31</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>49</v>
@@ -1404,15 +1321,15 @@
         <v>52</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>49</v>
@@ -1421,252 +1338,234 @@
         <v>52</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E45" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>35</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>36</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>37</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A46" s="1">
-        <v>34</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E46" s="1" t="s">
+    <row r="50" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>38</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="1">
-        <v>35</v>
-      </c>
-      <c r="B48" s="1" t="s">
+    <row r="52" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>39</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>40</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="1">
-        <v>36</v>
-      </c>
-      <c r="B49" s="1" t="s">
+      <c r="D53" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>41</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="1">
-        <v>37</v>
-      </c>
-      <c r="B50" s="1" t="s">
+      <c r="D54" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>42</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="1">
-        <v>38</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E51" s="1" t="s">
+      <c r="D55" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="1">
-        <v>39</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="1">
-        <v>40</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="1">
-        <v>41</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="1">
-        <v>42</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>43</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C60" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>47</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D60" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A61" s="1">
-        <v>46</v>
-      </c>
-      <c r="B61" s="1" t="s">
+      <c r="D61" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D61" s="1" t="s">
+      <c r="E61" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A62" s="1">
-        <v>47</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated ablaufplan and systemtest.
</commit_message>
<xml_diff>
--- a/Testdokumente/systemtest.xlsx
+++ b/Testdokumente/systemtest.xlsx
@@ -62,12 +62,6 @@
     <t>Einloggen als Wähler</t>
   </si>
   <si>
-    <t>Öffnen der Software -&gt; Fingerabdruck scannen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Öffnen der Software -&gt; Fingerabdruck scannen </t>
-  </si>
-  <si>
     <t>Moderator: Wahl wurde angelegt, nun muss sie vom Wahlleiter freigegeben werden                                                                                                                                               Wahlleiter: Wahl wurde angelegt</t>
   </si>
   <si>
@@ -239,15 +233,6 @@
     <t>Wähler hat ungültige Stimme abgegeben. Zurück zur Startseite und diese Wahl wird dem Wähler nicht mehr angezeigt.</t>
   </si>
   <si>
-    <t>Bundestagswahl aus Liste der verfügbaren Wahlen auswählen -&gt; Erststimme abgeben -&gt; Zweitstimme abgeben -&gt; Button "Auswahl bestätigen" anklicken -&gt; Button "Ja" anklicken</t>
-  </si>
-  <si>
-    <t>Europawahl aus Liste der verfügbaren Wahlen auswählen -&gt; Stimme abgeben -&gt; Button "Auswahl bestätigen" anklicken -&gt; Button "Ja" anklicken</t>
-  </si>
-  <si>
-    <t>Bürgermeisterwahl aus Liste der verfügbaren Wahlen auswählen -&gt; Stimme mehrfach oder gar nicht abgeben -&gt; Button "Auswahl bestätigen" anklicken -&gt; Button "Ja" anklicken</t>
-  </si>
-  <si>
     <t>Europawahl anlegen (Moderator/Wahlleiter)</t>
   </si>
   <si>
@@ -368,27 +353,6 @@
     <t>Bei einer beendeten Wahl Button "Auswerten" anklicken -&gt; Werte auf Korrektheit prüfen -&gt; Werte nicht korrekt</t>
   </si>
   <si>
-    <t>Bürgerentscheid aus Liste der verfügbaren Wahlen auswählen -&gt; Stimme abgeben -&gt; Button "Auswahl bestätigen" anklicken -&gt; Button "Ja" anklicken</t>
-  </si>
-  <si>
-    <t>Landratswahl aus Liste der verfügbaren Wahlen auswählen -&gt; Stimme abgeben -&gt; Button "Auswahl bestätigen" anklicken -&gt; Button "Ja" anklicken</t>
-  </si>
-  <si>
-    <t>Bundestagswahl aus Liste der verfügbaren Wahlen auswählen -&gt; Button "Stimme ungültig machen" anklicken -&gt; Button "Ja" anklicken</t>
-  </si>
-  <si>
-    <t>Europawahl aus Liste der verfügbaren Wahlen auswählen -&gt; Button "Stimme ungültig machen" anklicken -&gt; Button "Ja" anklicken</t>
-  </si>
-  <si>
-    <t>Bürgerentscheid aus Liste der verfügbaren Wahlen auswählen -&gt; Button "Stimme ungültig machen" anklicken -&gt; Button "Ja" anklicken</t>
-  </si>
-  <si>
-    <t>Landratswahl aus Liste der verfügbaren Wahlen auswählen -&gt; Button "Stimme ungültig machen" anklicken -&gt; Button "Ja" anklicken</t>
-  </si>
-  <si>
-    <t>Bürgermeisterwahl aus Liste der verfügbaren Wahlen auswählen -&gt; Button "Stimme ungültig machen" anklicken -&gt; Button "Ja" anklicken</t>
-  </si>
-  <si>
     <t>Wahl ist freigegeben und ist somit ab dem entsprechenden Datum für die Wähler zugänglich. Es können weitere Wahlen freigegeben/gelöscht werden.</t>
   </si>
   <si>
@@ -401,7 +365,43 @@
     <t>Login schlägt fehl und Fehlermeldung wird angezeigt. "Falsche Login-Daten"</t>
   </si>
   <si>
-    <t>Login schlägt fehl und Fehlermeldung wird angezeigt. "Fingerabdruck nicht registriert"</t>
+    <t>Öffnen der Software -&gt; Login-Daten eingeben -&gt; RFID-Tag einlesen</t>
+  </si>
+  <si>
+    <t>Öffnen der Software -&gt; Falsche Login-Daten eingeben -&gt; RFID-Tag einlesen</t>
+  </si>
+  <si>
+    <t>Login schlägt fehl und Fehlermeldung wird angezeigt. "Falsche Login Daten"</t>
+  </si>
+  <si>
+    <t>Bundestagswahl aus Liste der verfügbaren Wahlen auswählen -&gt; Erststimme abgeben -&gt; Zweitstimme abgeben -&gt; Button "Auswahl bestätigen" anklicken -&gt; RFID-Tag einscannen -&gt; "Bestätigen" anklicken</t>
+  </si>
+  <si>
+    <t>Bundestagswahl aus Liste der verfügbaren Wahlen auswählen -&gt; Button "Stimme ungültig machen" anklicken -&gt; RFID-Tag einscannen -&gt; "Bestätigen" anklicken</t>
+  </si>
+  <si>
+    <t>Europawahl aus Liste der verfügbaren Wahlen auswählen -&gt; Stimme abgeben -&gt; Button "Auswahl bestätigen" anklicken -&gt; RFID-Tag einscannen -&gt; "Bestätigen" anklicken</t>
+  </si>
+  <si>
+    <t>Europawahl aus Liste der verfügbaren Wahlen auswählen -&gt; Button "Stimme ungültig machen" anklicken -&gt; RFID-Tag einscannen -&gt; "Bestätigen" anklicken</t>
+  </si>
+  <si>
+    <t>Bürgerentscheid aus Liste der verfügbaren Wahlen auswählen -&gt; Stimme abgeben -&gt; Button "Auswahl bestätigen" anklicken -&gt; RFID-Tag einscannen -&gt; "Bestätigen" anklicken</t>
+  </si>
+  <si>
+    <t>Bürgerentscheid aus Liste der verfügbaren Wahlen auswählen -&gt; Button "Stimme ungültig machen" anklicken -&gt; RFID-Tag einscannen -&gt; "Bestätigen" anklicken</t>
+  </si>
+  <si>
+    <t>Landratswahl aus Liste der verfügbaren Wahlen auswählen -&gt; Stimme abgeben -&gt; Button "Auswahl bestätigen" anklicken -&gt; RFID-Tag einscannen -&gt; "Bestätigen" anklicken</t>
+  </si>
+  <si>
+    <t>Landratswahl aus Liste der verfügbaren Wahlen auswählen -&gt; Button "Stimme ungültig machen" anklicken -&gt; RFID-Tag einscannen -&gt; "Bestätigen" anklicken</t>
+  </si>
+  <si>
+    <t>Bürgermeisterwahl aus Liste der verfügbaren Wahlen auswählen -&gt; Stimme mehrfach oder gar nicht abgeben -&gt; Button "Auswahl bestätigen" anklicken -&gt; RFID-Tag einscannen -&gt; "Bestätigen" anklicken</t>
+  </si>
+  <si>
+    <t>Bürgermeisterwahl aus Liste der verfügbaren Wahlen auswählen -&gt; Button "Stimme ungültig machen" anklicken -&gt; RFID-Tag einscannen -&gt; "Bestätigen" anklicken</t>
   </si>
 </sst>
 </file>
@@ -752,8 +752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="D17" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="37.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,7 +797,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -814,7 +814,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -828,13 +828,13 @@
         <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -845,10 +845,10 @@
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>113</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -856,16 +856,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -873,16 +873,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -890,16 +890,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -907,16 +907,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -924,16 +924,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -941,16 +941,16 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -958,16 +958,16 @@
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="D14" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -975,16 +975,16 @@
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D15" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -992,16 +992,16 @@
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1009,16 +1009,16 @@
         <v>14</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="E19" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1026,16 +1026,16 @@
         <v>15</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="E20" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1043,16 +1043,16 @@
         <v>16</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1060,16 +1060,16 @@
         <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1077,16 +1077,16 @@
         <v>19</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>71</v>
+        <v>117</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1094,33 +1094,33 @@
         <v>20</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="D26" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>21</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1128,33 +1128,33 @@
         <v>22</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="D29" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>23</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1162,16 +1162,16 @@
         <v>24</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="D32" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1179,16 +1179,16 @@
         <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>72</v>
+        <v>123</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1196,16 +1196,16 @@
         <v>26</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="D35" s="1" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1213,16 +1213,16 @@
         <v>27</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1230,16 +1230,16 @@
         <v>28</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="D38" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1247,16 +1247,16 @@
         <v>29</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="D39" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1264,16 +1264,16 @@
         <v>30</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="D40" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1281,16 +1281,16 @@
         <v>31</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="E42" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1298,16 +1298,16 @@
         <v>32</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1315,16 +1315,16 @@
         <v>33</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="E44" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1332,16 +1332,16 @@
         <v>34</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -1349,16 +1349,16 @@
         <v>35</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1366,16 +1366,16 @@
         <v>36</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1383,16 +1383,16 @@
         <v>37</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1400,16 +1400,16 @@
         <v>38</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -1417,16 +1417,16 @@
         <v>39</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1434,16 +1434,16 @@
         <v>40</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1451,16 +1451,16 @@
         <v>41</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="E54" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1468,16 +1468,16 @@
         <v>42</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1485,16 +1485,16 @@
         <v>43</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1502,16 +1502,16 @@
         <v>44</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1519,16 +1519,16 @@
         <v>45</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1536,16 +1536,16 @@
         <v>46</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1553,16 +1553,16 @@
         <v>47</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="E61" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>